<commit_message>
Added TestCases for Product details page & added description for each test method
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9719429-44D0-4C99-8031-62003CE4528D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533D988-405F-414E-B67C-E4F6C497FE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -97,6 +97,24 @@
   </si>
   <si>
     <t xml:space="preserve">Verify user is able to search product </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Dashboard Page </t>
+  </si>
+  <si>
+    <t>Dashboard Page -&gt; Product listing page</t>
+  </si>
+  <si>
+    <t>product details page</t>
+  </si>
+  <si>
+    <t>verify page title on product details page</t>
+  </si>
+  <si>
+    <t>verify user redirects to correct details page</t>
+  </si>
+  <si>
+    <t>Sanity, Regression</t>
   </si>
 </sst>
 </file>
@@ -449,15 +467,16 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E9" sqref="E9"/>
+      <selection activeCell="C16" sqref="C16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="16.6640625" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" customWidth="1"/>
     <col min="2" max="2" width="17.21875" customWidth="1"/>
     <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="5" width="12.77734375" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" customWidth="1"/>
+    <col min="5" max="5" width="20" customWidth="1"/>
     <col min="6" max="6" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
@@ -531,7 +550,7 @@
         <v>17</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>21</v>
+        <v>29</v>
       </c>
       <c r="F4" s="2"/>
     </row>
@@ -581,7 +600,7 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="2" t="s">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>8</v>
@@ -599,7 +618,7 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="2" t="s">
-        <v>12</v>
+        <v>25</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>22</v>
@@ -632,19 +651,39 @@
       <c r="F11" s="2"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2"/>
-      <c r="B12" s="2"/>
-      <c r="C12" s="2"/>
-      <c r="D12" s="2"/>
-      <c r="E12" s="2"/>
+      <c r="A12" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B12" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="C12" s="2" t="s">
+        <v>27</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E12" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F12" s="2"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2"/>
-      <c r="B13" s="2"/>
-      <c r="C13" s="2"/>
-      <c r="D13" s="2"/>
-      <c r="E13" s="2"/>
+      <c r="A13" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B13" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C13" s="2" t="s">
+        <v>28</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="2" t="s">
+        <v>20</v>
+      </c>
       <c r="F13" s="2"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added YourOrdersPage & Test file
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D533D988-405F-414E-B67C-E4F6C497FE56}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C26BBB-E4DC-4ADD-9DDF-F5BEE18A58D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -115,13 +115,40 @@
   </si>
   <si>
     <t>Sanity, Regression</t>
+  </si>
+  <si>
+    <t>Shopping cart</t>
+  </si>
+  <si>
+    <t>Select a product and add it to the shopping cart.</t>
+  </si>
+  <si>
+    <t>Apply coupon code or promotional code</t>
+  </si>
+  <si>
+    <t>Select the delivery date</t>
+  </si>
+  <si>
+    <t>View the final order details including cost, and number of each product ordered. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Check if user is able to edit card details in amazon page </t>
+  </si>
+  <si>
+    <t>Edit Quantity cart boundary values</t>
+  </si>
+  <si>
+    <t>Select a single item and click the Delete link. </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Buy Now </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -133,6 +160,18 @@
       <b/>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Times New Roman"/>
+      <family val="1"/>
+    </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
       <name val="Times New Roman"/>
       <family val="1"/>
     </font>
@@ -178,12 +217,23 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
+      <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -464,23 +514,24 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F21"/>
+  <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16"/>
+      <selection sqref="A1:F28"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="36.88671875" customWidth="1"/>
-    <col min="2" max="2" width="17.21875" customWidth="1"/>
-    <col min="3" max="3" width="43.6640625" customWidth="1"/>
-    <col min="4" max="4" width="12.77734375" customWidth="1"/>
-    <col min="5" max="5" width="20" customWidth="1"/>
-    <col min="6" max="6" width="15.21875" customWidth="1"/>
+    <col min="1" max="1" width="36.88671875" style="2" customWidth="1"/>
+    <col min="2" max="2" width="17.21875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="74.6640625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="12.77734375" style="2" customWidth="1"/>
+    <col min="5" max="5" width="20" style="2" customWidth="1"/>
+    <col min="6" max="6" width="15.21875" style="2" customWidth="1"/>
+    <col min="7" max="16384" width="10.5546875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" ht="15.6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>4</v>
       </c>
@@ -501,254 +552,334 @@
       </c>
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B2" s="2" t="s">
+      <c r="B2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D2" s="2" t="s">
+      <c r="D2" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E2" s="2" t="s">
+      <c r="E2" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F2" s="2"/>
+      <c r="F2" s="3"/>
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B3" s="2" t="s">
+      <c r="B3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>10</v>
       </c>
-      <c r="D3" s="2" t="s">
+      <c r="D3" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="E3" s="2" t="s">
+      <c r="E3" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F3" s="2"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A4" s="2" t="s">
+      <c r="A4" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="B4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="2" t="s">
+      <c r="D4" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E4" s="2" t="s">
+      <c r="E4" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F4" s="2"/>
+      <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="2"/>
-      <c r="E5" s="2"/>
-      <c r="F5" s="2"/>
+      <c r="A5" s="3"/>
+      <c r="B5" s="3"/>
+      <c r="C5" s="3"/>
+      <c r="D5" s="3"/>
+      <c r="E5" s="3"/>
+      <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="2" t="s">
+      <c r="A6" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B6" s="2" t="s">
+      <c r="B6" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="D6" s="2" t="s">
+      <c r="D6" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E6" s="2" t="s">
+      <c r="E6" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F6" s="2"/>
+      <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A7" s="2" t="s">
+      <c r="A7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="B7" s="2" t="s">
+      <c r="B7" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="D7" s="2" t="s">
+      <c r="D7" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E7" s="2" t="s">
+      <c r="E7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F7" s="2"/>
+      <c r="F7" s="3"/>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A8" s="2" t="s">
+      <c r="A8" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="B8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="D8" s="2" t="s">
+      <c r="D8" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="E8" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F8" s="2"/>
+      <c r="F8" s="3"/>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A9" s="2" t="s">
+      <c r="A9" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B9" s="2" t="s">
+      <c r="B9" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C9" s="2" t="s">
+      <c r="C9" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D9" s="2" t="s">
+      <c r="D9" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E9" s="2" t="s">
+      <c r="E9" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F9" s="2"/>
+      <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="2"/>
-      <c r="B10" s="2"/>
-      <c r="C10" s="2"/>
-      <c r="D10" s="2"/>
-      <c r="E10" s="2"/>
-      <c r="F10" s="2"/>
+      <c r="A10" s="3"/>
+      <c r="B10" s="3"/>
+      <c r="C10" s="3"/>
+      <c r="D10" s="3"/>
+      <c r="E10" s="3"/>
+      <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="2"/>
-      <c r="B11" s="2"/>
-      <c r="C11" s="2"/>
-      <c r="D11" s="2"/>
-      <c r="E11" s="2"/>
-      <c r="F11" s="2"/>
+      <c r="A11" s="3"/>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="2" t="s">
+      <c r="A12" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B12" s="2" t="s">
+      <c r="B12" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="C12" s="2" t="s">
+      <c r="C12" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="D12" s="2" t="s">
+      <c r="D12" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E12" s="2" t="s">
+      <c r="E12" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F12" s="2"/>
+      <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A13" s="2" t="s">
+      <c r="A13" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B13" s="2" t="s">
+      <c r="B13" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="2" t="s">
+      <c r="C13" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="2" t="s">
+      <c r="D13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="E13" s="2" t="s">
+      <c r="E13" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="F13" s="2"/>
+      <c r="F13" s="3"/>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="2"/>
-      <c r="B14" s="2"/>
-      <c r="C14" s="2"/>
-      <c r="D14" s="2"/>
-      <c r="E14" s="2"/>
-      <c r="F14" s="2"/>
+      <c r="A14" s="3"/>
+      <c r="B14" s="3"/>
+      <c r="C14" s="3"/>
+      <c r="D14" s="3"/>
+      <c r="E14" s="3"/>
+      <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="2"/>
-      <c r="B15" s="2"/>
-      <c r="C15" s="2"/>
-      <c r="D15" s="2"/>
-      <c r="E15" s="2"/>
-      <c r="F15" s="2"/>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
+      <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="2"/>
-      <c r="B16" s="2"/>
-      <c r="C16" s="2"/>
-      <c r="D16" s="2"/>
-      <c r="E16" s="2"/>
-      <c r="F16" s="2"/>
+      <c r="A16" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B16" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C16" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
+      <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A17" s="2"/>
-      <c r="B17" s="2"/>
-      <c r="C17" s="2"/>
-      <c r="D17" s="2"/>
-      <c r="E17" s="2"/>
-      <c r="F17" s="2"/>
+      <c r="A17" s="3"/>
+      <c r="B17" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C17" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D17" s="3"/>
+      <c r="E17" s="3"/>
+      <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A18" s="2"/>
-      <c r="B18" s="2"/>
-      <c r="C18" s="2"/>
-      <c r="D18" s="2"/>
-      <c r="E18" s="2"/>
-      <c r="F18" s="2"/>
+      <c r="A18" s="3"/>
+      <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="D18" s="3"/>
+      <c r="E18" s="3"/>
+      <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="2"/>
-      <c r="B19" s="2"/>
-      <c r="C19" s="2"/>
-      <c r="D19" s="2"/>
-      <c r="E19" s="2"/>
-      <c r="F19" s="2"/>
+      <c r="A19" s="3"/>
+      <c r="B19" s="3"/>
+      <c r="C19" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="D19" s="3"/>
+      <c r="E19" s="3"/>
+      <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="2"/>
-      <c r="B20" s="2"/>
-      <c r="C20" s="2"/>
-      <c r="D20" s="2"/>
-      <c r="E20" s="2"/>
-      <c r="F20" s="2"/>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
+      <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="2"/>
-      <c r="B21" s="2"/>
-      <c r="C21" s="2"/>
-      <c r="D21" s="2"/>
-      <c r="E21" s="2"/>
-      <c r="F21" s="2"/>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
+      <c r="F21" s="3"/>
+    </row>
+    <row r="22" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A22" s="3"/>
+      <c r="B22" s="3"/>
+      <c r="C22" s="4" t="s">
+        <v>37</v>
+      </c>
+      <c r="D22" s="3"/>
+      <c r="E22" s="3"/>
+      <c r="F22" s="3"/>
+    </row>
+    <row r="23" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A23" s="3"/>
+      <c r="B23" s="3"/>
+      <c r="C23" s="3"/>
+      <c r="D23" s="3"/>
+      <c r="E23" s="3"/>
+      <c r="F23" s="3"/>
+    </row>
+    <row r="24" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A24" s="3"/>
+      <c r="B24" s="3"/>
+      <c r="C24" s="3"/>
+      <c r="D24" s="3"/>
+      <c r="E24" s="3"/>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="B25" s="3"/>
+      <c r="C25" s="3"/>
+      <c r="D25" s="3"/>
+      <c r="E25" s="3"/>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3"/>
+      <c r="B26" s="3"/>
+      <c r="C26" s="3"/>
+      <c r="D26" s="3"/>
+      <c r="E26" s="3"/>
+      <c r="F26" s="3"/>
+    </row>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
+      <c r="B27" s="3"/>
+      <c r="C27" s="3"/>
+      <c r="D27" s="3"/>
+      <c r="E27" s="3"/>
+      <c r="F27" s="3"/>
+    </row>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
+      <c r="B28" s="3"/>
+      <c r="C28" s="3"/>
+      <c r="D28" s="3"/>
+      <c r="E28" s="3"/>
+      <c r="F28" s="3"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added all test implementation for shopping cart
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7C26BBB-E4DC-4ADD-9DDF-F5BEE18A58D1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29BED7D-7E52-447E-AD02-D7203E71F942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -517,7 +517,7 @@
   <dimension ref="A1:F28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection sqref="A1:F28"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Implemented test case which adds product to shoppingcart
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D29BED7D-7E52-447E-AD02-D7203E71F942}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A838380-78A7-4502-9879-798EBBF335FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="63" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t xml:space="preserve">Buy Now </t>
+  </si>
+  <si>
+    <t xml:space="preserve">YourOrders Page </t>
+  </si>
+  <si>
+    <t>Regression, Sanity</t>
   </si>
 </sst>
 </file>
@@ -514,10 +520,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F28"/>
+  <dimension ref="A1:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C21" sqref="C21"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -746,121 +752,163 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="3" t="s">
-        <v>30</v>
+        <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="4" t="s">
-        <v>31</v>
-      </c>
-      <c r="D16" s="3"/>
-      <c r="E16" s="3"/>
+        <v>7</v>
+      </c>
+      <c r="C16" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="D16" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>40</v>
+      </c>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3"/>
-      <c r="B17" s="3" t="s">
-        <v>7</v>
-      </c>
-      <c r="C17" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="B17" s="3"/>
+      <c r="C17" s="3"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3"/>
-      <c r="B18" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C18" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="B18" s="3"/>
+      <c r="C18" s="3"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="4" t="s">
-        <v>34</v>
-      </c>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
+      <c r="A19" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B19" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
+      <c r="A20" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B20" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C20" s="3" t="s">
-        <v>35</v>
-      </c>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
+        <v>28</v>
+      </c>
+      <c r="D20" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3"/>
-      <c r="B21" s="3"/>
-      <c r="C21" s="3" t="s">
-        <v>36</v>
+      <c r="A21" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B21" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C21" s="4" t="s">
+        <v>31</v>
       </c>
       <c r="D21" s="3"/>
       <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A22" s="3"/>
+      <c r="A22" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B22" s="3"/>
-      <c r="C22" s="4" t="s">
-        <v>37</v>
+      <c r="C22" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D22" s="3"/>
       <c r="E22" s="3"/>
       <c r="F22" s="3"/>
     </row>
     <row r="23" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A23" s="3"/>
+      <c r="A23" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B23" s="3"/>
-      <c r="C23" s="3"/>
+      <c r="C23" s="5" t="s">
+        <v>33</v>
+      </c>
       <c r="D23" s="3"/>
       <c r="E23" s="3"/>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B24" s="3"/>
-      <c r="C24" s="3"/>
+      <c r="C24" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A25" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="3"/>
+      <c r="C25" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3"/>
+      <c r="C26" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
@@ -868,19 +916,47 @@
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="3"/>
+      <c r="C27" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B28" s="3"/>
       <c r="C28" s="3"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
+    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A29" s="3"/>
+      <c r="B29" s="3"/>
+      <c r="C29" s="3"/>
+      <c r="D29" s="3"/>
+      <c r="E29" s="3"/>
+      <c r="F29" s="3"/>
+    </row>
+    <row r="30" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A30" s="3"/>
+      <c r="B30" s="3"/>
+      <c r="C30" s="3"/>
+      <c r="D30" s="3"/>
+      <c r="E30" s="3"/>
+      <c r="F30" s="3"/>
+    </row>
+    <row r="31" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A31" s="3"/>
+      <c r="B31" s="3"/>
+      <c r="C31" s="3"/>
+      <c r="D31" s="3"/>
+      <c r="E31" s="3"/>
+      <c r="F31" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated test cases sheet & test file descriptions
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4A838380-78A7-4502-9879-798EBBF335FE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{35C0993E-427D-4FB1-8356-5379BF684855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="86" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="41">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -523,7 +523,7 @@
   <dimension ref="A1:F31"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="C21" sqref="C21"/>
+      <selection activeCell="A22" sqref="A22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -849,8 +849,12 @@
       <c r="C21" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="D21" s="3"/>
-      <c r="E21" s="3"/>
+      <c r="D21" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E21" s="3" t="s">
+        <v>29</v>
+      </c>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
test case sheet updated
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{65BAE198-DFF7-4F3F-8B79-E48F7FE21F39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46D9105-4E20-4D3A-AD5C-686BEB7EF687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -154,6 +154,9 @@
   </si>
   <si>
     <t>Check correct page path is getting shown</t>
+  </si>
+  <si>
+    <t>List of products added into shopping cart</t>
   </si>
 </sst>
 </file>
@@ -526,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F32"/>
+  <dimension ref="A1:F33"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E19" sqref="E19"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -895,12 +898,18 @@
       <c r="A23" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B23" s="3"/>
-      <c r="C23" s="5" t="s">
-        <v>32</v>
-      </c>
-      <c r="D23" s="3"/>
-      <c r="E23" s="3"/>
+      <c r="B23" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C23" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D23" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E23" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
@@ -909,7 +918,7 @@
       </c>
       <c r="B24" s="3"/>
       <c r="C24" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
@@ -920,8 +929,8 @@
         <v>30</v>
       </c>
       <c r="B25" s="3"/>
-      <c r="C25" s="4" t="s">
-        <v>34</v>
+      <c r="C25" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
@@ -932,8 +941,8 @@
         <v>30</v>
       </c>
       <c r="B26" s="3"/>
-      <c r="C26" s="3" t="s">
-        <v>35</v>
+      <c r="C26" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
@@ -945,34 +954,38 @@
       </c>
       <c r="B27" s="3"/>
       <c r="C27" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
     <row r="28" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A28" s="3"/>
+      <c r="A28" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="4" t="s">
-        <v>37</v>
+      <c r="C28" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A29" s="3"/>
       <c r="B29" s="3"/>
-      <c r="C29" s="3"/>
+      <c r="C29" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
       <c r="F29" s="3"/>
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A30" s="3"/>
+      <c r="A30" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B30" s="3"/>
       <c r="C30" s="3"/>
       <c r="D30" s="3"/>
@@ -995,6 +1008,14 @@
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
+    <row r="33" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A33" s="3"/>
+      <c r="B33" s="3"/>
+      <c r="C33" s="3"/>
+      <c r="D33" s="3"/>
+      <c r="E33" s="3"/>
+      <c r="F33" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
implemented proceed to chekout flow
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E46D9105-4E20-4D3A-AD5C-686BEB7EF687}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9193B70D-EFAB-48EB-8390-54DE9F96FF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -529,10 +529,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F33"/>
+  <dimension ref="A1:F36"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -913,48 +913,36 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A24" s="3"/>
       <c r="B24" s="3"/>
-      <c r="C24" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="C24" s="4"/>
       <c r="D24" s="3"/>
       <c r="E24" s="3"/>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A25" s="3"/>
       <c r="B25" s="3"/>
-      <c r="C25" s="5" t="s">
-        <v>33</v>
-      </c>
+      <c r="C25" s="4"/>
       <c r="D25" s="3"/>
       <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>30</v>
-      </c>
+      <c r="A26" s="3"/>
       <c r="B26" s="3"/>
-      <c r="C26" s="4" t="s">
-        <v>34</v>
-      </c>
+      <c r="C26" s="4"/>
       <c r="D26" s="3"/>
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B27" s="3"/>
-      <c r="C27" s="3" t="s">
-        <v>35</v>
+      <c r="C27" s="5" t="s">
+        <v>32</v>
       </c>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
@@ -965,18 +953,20 @@
         <v>30</v>
       </c>
       <c r="B28" s="3"/>
-      <c r="C28" s="3" t="s">
-        <v>36</v>
+      <c r="C28" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
     <row r="29" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A29" s="3"/>
+      <c r="A29" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B29" s="3"/>
       <c r="C29" s="4" t="s">
-        <v>37</v>
+        <v>34</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -984,18 +974,24 @@
     </row>
     <row r="30" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A30" s="3" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3"/>
+      <c r="C30" s="3" t="s">
+        <v>35</v>
+      </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
       <c r="F30" s="3"/>
     </row>
     <row r="31" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A31" s="3"/>
+      <c r="A31" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3"/>
+      <c r="C31" s="3" t="s">
+        <v>36</v>
+      </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
@@ -1003,19 +999,47 @@
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A32" s="3"/>
       <c r="B32" s="3"/>
-      <c r="C32" s="3"/>
+      <c r="C32" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B33" s="3"/>
       <c r="C33" s="3"/>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
+    <row r="34" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A34" s="3"/>
+      <c r="B34" s="3"/>
+      <c r="C34" s="3"/>
+      <c r="D34" s="3"/>
+      <c r="E34" s="3"/>
+      <c r="F34" s="3"/>
+    </row>
+    <row r="35" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A35" s="3"/>
+      <c r="B35" s="3"/>
+      <c r="C35" s="3"/>
+      <c r="D35" s="3"/>
+      <c r="E35" s="3"/>
+      <c r="F35" s="3"/>
+    </row>
+    <row r="36" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A36" s="3"/>
+      <c r="B36" s="3"/>
+      <c r="C36" s="3"/>
+      <c r="D36" s="3"/>
+      <c r="E36" s="3"/>
+      <c r="F36" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
updated test cases sheet with shoppng cart page
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9193B70D-EFAB-48EB-8390-54DE9F96FF8F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426FADC-13EA-4241-ABFF-AD91DD05F95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="103" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -157,6 +157,12 @@
   </si>
   <si>
     <t>List of products added into shopping cart</t>
+  </si>
+  <si>
+    <t>TC5</t>
+  </si>
+  <si>
+    <t>Check if user is able to proceed to checkout</t>
   </si>
 </sst>
 </file>
@@ -532,7 +538,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -913,11 +919,21 @@
       <c r="F23" s="3"/>
     </row>
     <row r="24" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A24" s="3"/>
-      <c r="B24" s="3"/>
-      <c r="C24" s="4"/>
-      <c r="D24" s="3"/>
-      <c r="E24" s="3"/>
+      <c r="A24" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B24" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>45</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>21</v>
+      </c>
       <c r="F24" s="3"/>
     </row>
     <row r="25" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
updated test case & test details
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0426FADC-13EA-4241-ABFF-AD91DD05F95C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B910BD-571C-4F9F-9A2C-BA5768B23999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="108" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -163,6 +163,9 @@
   </si>
   <si>
     <t>Check if user is able to proceed to checkout</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Verify user profile details name on all section </t>
   </si>
 </sst>
 </file>
@@ -538,7 +541,7 @@
   <dimension ref="A1:F36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C10" sqref="C10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -707,11 +710,21 @@
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A10" s="3"/>
-      <c r="B10" s="3"/>
-      <c r="C10" s="3"/>
-      <c r="D10" s="3"/>
-      <c r="E10" s="3"/>
+      <c r="A10" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>44</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F10" s="3"/>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Added Test for create account on login page
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87B910BD-571C-4F9F-9A2C-BA5768B23999}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A92949E-7FEA-4E69-AD48-9D9814FBF5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="113" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="48">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -166,6 +166,9 @@
   </si>
   <si>
     <t xml:space="preserve">Verify user profile details name on all section </t>
+  </si>
+  <si>
+    <t>Verify Create_account option in login page</t>
   </si>
 </sst>
 </file>
@@ -538,10 +541,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F36"/>
+  <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C10" sqref="C10"/>
+      <selection activeCell="E6" sqref="E6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -630,29 +633,29 @@
       <c r="F4" s="3"/>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A5" s="3"/>
-      <c r="B5" s="3"/>
-      <c r="C5" s="3"/>
-      <c r="D5" s="3"/>
-      <c r="E5" s="3"/>
+      <c r="A5" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="B5" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C5" s="3" t="s">
+        <v>47</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F5" s="3"/>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A6" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="B6" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="D6" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E6" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A6" s="3"/>
+      <c r="B6" s="3"/>
+      <c r="C6" s="3"/>
+      <c r="D6" s="3"/>
+      <c r="E6" s="3"/>
       <c r="F6" s="3"/>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.3">
@@ -660,10 +663,10 @@
         <v>12</v>
       </c>
       <c r="B7" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C7" s="3" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="D7" s="3" t="s">
         <v>18</v>
@@ -675,13 +678,13 @@
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="3" t="s">
-        <v>24</v>
+        <v>12</v>
       </c>
       <c r="B8" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C8" s="3" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D8" s="3" t="s">
         <v>18</v>
@@ -693,64 +696,64 @@
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="3" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C9" s="3" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="D9" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E9" s="3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="F9" s="3"/>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="B10" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C10" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E10" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="F10" s="3"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A11" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B11" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C10" s="3" t="s">
+      <c r="C11" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="D10" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E10" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F10" s="3"/>
-    </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A11" s="3"/>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
+      <c r="D11" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E11" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F11" s="3"/>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A12" s="3" t="s">
-        <v>26</v>
-      </c>
-      <c r="B12" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C12" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D12" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E12" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A12" s="3"/>
+      <c r="B12" s="3"/>
+      <c r="C12" s="3"/>
+      <c r="D12" s="3"/>
+      <c r="E12" s="3"/>
       <c r="F12" s="3"/>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.3">
@@ -758,43 +761,43 @@
         <v>26</v>
       </c>
       <c r="B13" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C13" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E13" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F13" s="3"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A14" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B14" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="C13" s="3" t="s">
+      <c r="C14" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="D13" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E13" s="3" t="s">
-        <v>20</v>
-      </c>
-      <c r="F13" s="3"/>
-    </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A14" s="3"/>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
-      <c r="D14" s="3"/>
-      <c r="E14" s="3"/>
+      <c r="D14" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B15" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C15" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D15" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E15" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A15" s="3"/>
+      <c r="B15" s="3"/>
+      <c r="C15" s="3"/>
+      <c r="D15" s="3"/>
+      <c r="E15" s="3"/>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
@@ -802,16 +805,16 @@
         <v>39</v>
       </c>
       <c r="B16" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C16" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D16" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E16" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F16" s="3"/>
     </row>
@@ -820,16 +823,16 @@
         <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -838,43 +841,43 @@
         <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C18" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F18" s="3"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A19" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B19" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="3" t="s">
+      <c r="C19" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D18" s="3" t="s">
+      <c r="D19" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E18" s="3" t="s">
+      <c r="E19" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F18" s="3"/>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A19" s="3"/>
-      <c r="B19" s="3"/>
-      <c r="C19" s="3"/>
-      <c r="D19" s="3"/>
-      <c r="E19" s="3"/>
       <c r="F19" s="3"/>
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B20" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C20" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D20" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E20" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A20" s="3"/>
+      <c r="B20" s="3"/>
+      <c r="C20" s="3"/>
+      <c r="D20" s="3"/>
+      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
@@ -882,10 +885,10 @@
         <v>30</v>
       </c>
       <c r="B21" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C21" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D21" s="3" t="s">
         <v>18</v>
@@ -900,16 +903,16 @@
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C22" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="C22" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D22" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E22" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F22" s="3"/>
     </row>
@@ -918,16 +921,16 @@
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C23" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -936,25 +939,35 @@
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C24" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D24" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E24" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F24" s="3"/>
+    </row>
+    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A25" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B25" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C24" s="4" t="s">
+      <c r="C25" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D24" s="3" t="s">
+      <c r="D25" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E24" s="3" t="s">
+      <c r="E25" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F24" s="3"/>
-    </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A25" s="3"/>
-      <c r="B25" s="3"/>
-      <c r="C25" s="4"/>
-      <c r="D25" s="3"/>
-      <c r="E25" s="3"/>
       <c r="F25" s="3"/>
     </row>
     <row r="26" spans="1:6" x14ac:dyDescent="0.3">
@@ -965,25 +978,21 @@
       <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
-    <row r="27" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A27" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="27" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A27" s="3"/>
       <c r="B27" s="3"/>
-      <c r="C27" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="C27" s="4"/>
       <c r="D27" s="3"/>
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A28" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B28" s="3"/>
       <c r="C28" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
@@ -994,8 +1003,8 @@
         <v>30</v>
       </c>
       <c r="B29" s="3"/>
-      <c r="C29" s="4" t="s">
-        <v>34</v>
+      <c r="C29" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1006,8 +1015,8 @@
         <v>30</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="3" t="s">
-        <v>35</v>
+      <c r="C30" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1019,34 +1028,38 @@
       </c>
       <c r="B31" s="3"/>
       <c r="C31" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
       <c r="F31" s="3"/>
     </row>
     <row r="32" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A32" s="3"/>
+      <c r="A32" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B32" s="3"/>
-      <c r="C32" s="4" t="s">
-        <v>37</v>
+      <c r="C32" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A33" s="3"/>
       <c r="B33" s="3"/>
-      <c r="C33" s="3"/>
+      <c r="C33" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3"/>
+      <c r="A34" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B34" s="3"/>
       <c r="C34" s="3"/>
       <c r="D34" s="3"/>
@@ -1069,6 +1082,14 @@
       <c r="E36" s="3"/>
       <c r="F36" s="3"/>
     </row>
+    <row r="37" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A37" s="3"/>
+      <c r="B37" s="3"/>
+      <c r="C37" s="3"/>
+      <c r="D37" s="3"/>
+      <c r="E37" s="3"/>
+      <c r="F37" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated test for dashboard page
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8A92949E-7FEA-4E69-AD48-9D9814FBF5B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65CE8F6-D0B1-4726-80EB-5CAB0E1E2EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -544,7 +544,7 @@
   <dimension ref="A1:F37"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E6" sqref="E6"/>
+      <selection activeCell="C12" sqref="C12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Updated Product details page test
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F65CE8F6-D0B1-4726-80EB-5CAB0E1E2EEE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CE7984-C3E6-486A-A12A-D8AC913177F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -169,6 +169,12 @@
   </si>
   <si>
     <t>Verify Create_account option in login page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Product Details Page </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fetching all product details </t>
   </si>
 </sst>
 </file>
@@ -541,10 +547,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:F37"/>
+  <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+      <selection activeCell="A15" sqref="A15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -793,29 +799,29 @@
       <c r="F14" s="3"/>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A15" s="3"/>
-      <c r="B15" s="3"/>
-      <c r="C15" s="3"/>
-      <c r="D15" s="3"/>
-      <c r="E15" s="3"/>
+      <c r="A15" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C15" s="3" t="s">
+        <v>49</v>
+      </c>
+      <c r="D15" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>20</v>
+      </c>
       <c r="F15" s="3"/>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A16" s="3" t="s">
-        <v>39</v>
-      </c>
-      <c r="B16" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C16" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D16" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E16" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A16" s="3"/>
+      <c r="B16" s="3"/>
+      <c r="C16" s="3"/>
+      <c r="D16" s="3"/>
+      <c r="E16" s="3"/>
       <c r="F16" s="3"/>
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
@@ -823,16 +829,16 @@
         <v>39</v>
       </c>
       <c r="B17" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C17" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D17" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E17" s="3" t="s">
-        <v>40</v>
+        <v>20</v>
       </c>
       <c r="F17" s="3"/>
     </row>
@@ -841,16 +847,16 @@
         <v>39</v>
       </c>
       <c r="B18" s="3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C18" s="3" t="s">
-        <v>41</v>
+        <v>28</v>
       </c>
       <c r="D18" s="3" t="s">
         <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="F18" s="3"/>
     </row>
@@ -859,43 +865,43 @@
         <v>39</v>
       </c>
       <c r="B19" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C19" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="D19" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F19" s="3"/>
+    </row>
+    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A20" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="C19" s="3" t="s">
+      <c r="C20" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="D19" s="3" t="s">
+      <c r="D20" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E19" s="3" t="s">
+      <c r="E20" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="F19" s="3"/>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A20" s="3"/>
-      <c r="B20" s="3"/>
-      <c r="C20" s="3"/>
-      <c r="D20" s="3"/>
-      <c r="E20" s="3"/>
       <c r="F20" s="3"/>
     </row>
     <row r="21" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A21" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="B21" s="3" t="s">
-        <v>6</v>
-      </c>
-      <c r="C21" s="3" t="s">
-        <v>27</v>
-      </c>
-      <c r="D21" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="E21" s="3" t="s">
-        <v>20</v>
-      </c>
+      <c r="A21" s="3"/>
+      <c r="B21" s="3"/>
+      <c r="C21" s="3"/>
+      <c r="D21" s="3"/>
+      <c r="E21" s="3"/>
       <c r="F21" s="3"/>
     </row>
     <row r="22" spans="1:6" x14ac:dyDescent="0.3">
@@ -903,10 +909,10 @@
         <v>30</v>
       </c>
       <c r="B22" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="C22" s="3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D22" s="3" t="s">
         <v>18</v>
@@ -921,16 +927,16 @@
         <v>30</v>
       </c>
       <c r="B23" s="3" t="s">
-        <v>8</v>
-      </c>
-      <c r="C23" s="4" t="s">
-        <v>31</v>
+        <v>7</v>
+      </c>
+      <c r="C23" s="3" t="s">
+        <v>28</v>
       </c>
       <c r="D23" s="3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="E23" s="3" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F23" s="3"/>
     </row>
@@ -939,16 +945,16 @@
         <v>30</v>
       </c>
       <c r="B24" s="3" t="s">
-        <v>22</v>
+        <v>8</v>
       </c>
       <c r="C24" s="4" t="s">
-        <v>43</v>
+        <v>31</v>
       </c>
       <c r="D24" s="3" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E24" s="3" t="s">
-        <v>20</v>
+        <v>29</v>
       </c>
       <c r="F24" s="3"/>
     </row>
@@ -957,25 +963,35 @@
         <v>30</v>
       </c>
       <c r="B25" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C25" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="D25" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="E25" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="F25" s="3"/>
+    </row>
+    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A26" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="B26" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="C25" s="4" t="s">
+      <c r="C26" s="4" t="s">
         <v>45</v>
       </c>
-      <c r="D25" s="3" t="s">
+      <c r="D26" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="E25" s="3" t="s">
+      <c r="E26" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="F25" s="3"/>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A26" s="3"/>
-      <c r="B26" s="3"/>
-      <c r="C26" s="4"/>
-      <c r="D26" s="3"/>
-      <c r="E26" s="3"/>
       <c r="F26" s="3"/>
     </row>
     <row r="27" spans="1:6" x14ac:dyDescent="0.3">
@@ -986,25 +1002,21 @@
       <c r="E27" s="3"/>
       <c r="F27" s="3"/>
     </row>
-    <row r="28" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="A28" s="3" t="s">
-        <v>30</v>
-      </c>
+    <row r="28" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A28" s="3"/>
       <c r="B28" s="3"/>
-      <c r="C28" s="5" t="s">
-        <v>32</v>
-      </c>
+      <c r="C28" s="4"/>
       <c r="D28" s="3"/>
       <c r="E28" s="3"/>
       <c r="F28" s="3"/>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:6" ht="16.2" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
       <c r="B29" s="3"/>
       <c r="C29" s="5" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="D29" s="3"/>
       <c r="E29" s="3"/>
@@ -1015,8 +1027,8 @@
         <v>30</v>
       </c>
       <c r="B30" s="3"/>
-      <c r="C30" s="4" t="s">
-        <v>34</v>
+      <c r="C30" s="5" t="s">
+        <v>33</v>
       </c>
       <c r="D30" s="3"/>
       <c r="E30" s="3"/>
@@ -1027,8 +1039,8 @@
         <v>30</v>
       </c>
       <c r="B31" s="3"/>
-      <c r="C31" s="3" t="s">
-        <v>35</v>
+      <c r="C31" s="4" t="s">
+        <v>34</v>
       </c>
       <c r="D31" s="3"/>
       <c r="E31" s="3"/>
@@ -1040,34 +1052,38 @@
       </c>
       <c r="B32" s="3"/>
       <c r="C32" s="3" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="D32" s="3"/>
       <c r="E32" s="3"/>
       <c r="F32" s="3"/>
     </row>
     <row r="33" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A33" s="3"/>
+      <c r="A33" s="3" t="s">
+        <v>30</v>
+      </c>
       <c r="B33" s="3"/>
-      <c r="C33" s="4" t="s">
-        <v>37</v>
+      <c r="C33" s="3" t="s">
+        <v>36</v>
       </c>
       <c r="D33" s="3"/>
       <c r="E33" s="3"/>
       <c r="F33" s="3"/>
     </row>
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A34" s="3" t="s">
-        <v>38</v>
-      </c>
+      <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="3"/>
+      <c r="C34" s="4" t="s">
+        <v>37</v>
+      </c>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A35" s="3"/>
+      <c r="A35" s="3" t="s">
+        <v>38</v>
+      </c>
       <c r="B35" s="3"/>
       <c r="C35" s="3"/>
       <c r="D35" s="3"/>
@@ -1090,6 +1106,14 @@
       <c r="E37" s="3"/>
       <c r="F37" s="3"/>
     </row>
+    <row r="38" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="A38" s="3"/>
+      <c r="B38" s="3"/>
+      <c r="C38" s="3"/>
+      <c r="D38" s="3"/>
+      <c r="E38" s="3"/>
+      <c r="F38" s="3"/>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Updated Your account page test & added chromeoptions arguments
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28227"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{26CE7984-C3E6-486A-A12A-D8AC913177F5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41892ED-5B13-48B9-9E77-A26975F5799C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="123" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -138,12 +138,6 @@
     <t>Edit Quantity cart boundary values</t>
   </si>
   <si>
-    <t>Select a single item and click the Delete link. </t>
-  </si>
-  <si>
-    <t xml:space="preserve">Buy Now </t>
-  </si>
-  <si>
     <t xml:space="preserve">YourOrders Page </t>
   </si>
   <si>
@@ -175,6 +169,12 @@
   </si>
   <si>
     <t xml:space="preserve">Fetching all product details </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Your Account Page </t>
+  </si>
+  <si>
+    <t>Verify User gets redirects to correct page</t>
   </si>
 </sst>
 </file>
@@ -549,8 +549,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F38"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="C28" sqref="C28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -646,7 +646,7 @@
         <v>22</v>
       </c>
       <c r="C5" s="3" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="D5" s="3" t="s">
         <v>16</v>
@@ -741,10 +741,10 @@
         <v>24</v>
       </c>
       <c r="B11" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="C11" s="3" t="s">
         <v>44</v>
-      </c>
-      <c r="C11" s="3" t="s">
-        <v>46</v>
       </c>
       <c r="D11" s="3" t="s">
         <v>18</v>
@@ -800,13 +800,13 @@
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="3" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C15" s="3" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="D15" s="3" t="s">
         <v>18</v>
@@ -826,7 +826,7 @@
     </row>
     <row r="17" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A17" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B17" s="3" t="s">
         <v>6</v>
@@ -844,7 +844,7 @@
     </row>
     <row r="18" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A18" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B18" s="3" t="s">
         <v>7</v>
@@ -856,19 +856,19 @@
         <v>18</v>
       </c>
       <c r="E18" s="3" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="F18" s="3"/>
     </row>
     <row r="19" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A19" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B19" s="3" t="s">
         <v>8</v>
       </c>
       <c r="C19" s="3" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="D19" s="3" t="s">
         <v>18</v>
@@ -880,13 +880,13 @@
     </row>
     <row r="20" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A20" s="3" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B20" s="3" t="s">
         <v>22</v>
       </c>
       <c r="C20" s="3" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="D20" s="3" t="s">
         <v>17</v>
@@ -966,7 +966,7 @@
         <v>22</v>
       </c>
       <c r="C25" s="4" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="D25" s="3" t="s">
         <v>18</v>
@@ -981,10 +981,10 @@
         <v>30</v>
       </c>
       <c r="B26" s="3" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C26" s="4" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="D26" s="3" t="s">
         <v>17</v>
@@ -1014,7 +1014,9 @@
       <c r="A29" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B29" s="3"/>
+      <c r="B29" s="3" t="s">
+        <v>6</v>
+      </c>
       <c r="C29" s="5" t="s">
         <v>32</v>
       </c>
@@ -1026,7 +1028,9 @@
       <c r="A30" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B30" s="3"/>
+      <c r="B30" s="3" t="s">
+        <v>7</v>
+      </c>
       <c r="C30" s="5" t="s">
         <v>33</v>
       </c>
@@ -1038,7 +1042,9 @@
       <c r="A31" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B31" s="3"/>
+      <c r="B31" s="3" t="s">
+        <v>8</v>
+      </c>
       <c r="C31" s="4" t="s">
         <v>34</v>
       </c>
@@ -1050,7 +1056,9 @@
       <c r="A32" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B32" s="3"/>
+      <c r="B32" s="3" t="s">
+        <v>22</v>
+      </c>
       <c r="C32" s="3" t="s">
         <v>35</v>
       </c>
@@ -1062,7 +1070,9 @@
       <c r="A33" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B33" s="3"/>
+      <c r="B33" s="3" t="s">
+        <v>42</v>
+      </c>
       <c r="C33" s="3" t="s">
         <v>36</v>
       </c>
@@ -1073,19 +1083,21 @@
     <row r="34" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A34" s="3"/>
       <c r="B34" s="3"/>
-      <c r="C34" s="4" t="s">
-        <v>37</v>
-      </c>
+      <c r="C34" s="4"/>
       <c r="D34" s="3"/>
       <c r="E34" s="3"/>
       <c r="F34" s="3"/>
     </row>
     <row r="35" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A35" s="3" t="s">
-        <v>38</v>
-      </c>
-      <c r="B35" s="3"/>
-      <c r="C35" s="3"/>
+        <v>48</v>
+      </c>
+      <c r="B35" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C35" s="3" t="s">
+        <v>49</v>
+      </c>
       <c r="D35" s="3"/>
       <c r="E35" s="3"/>
       <c r="F35" s="3"/>

</xml_diff>

<commit_message>
Updated test cases sheet & deleted old test recording
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases Sheet.xlsx
+++ b/TestCases/Test Cases Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Automation_Framework\POM\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E41892ED-5B13-48B9-9E77-A26975F5799C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8825CC25-A73A-4C5D-B8DB-975CE241AFFA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="50">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="136" uniqueCount="53">
   <si>
     <t>Test Case ID</t>
   </si>
@@ -175,6 +175,15 @@
   </si>
   <si>
     <t>Verify User gets redirects to correct page</t>
+  </si>
+  <si>
+    <t>Verify all the options from your accounts page</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sanity </t>
+  </si>
+  <si>
+    <t xml:space="preserve">High </t>
   </si>
 </sst>
 </file>
@@ -550,7 +559,7 @@
   <dimension ref="A1:F38"/>
   <sheetViews>
     <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="C28" sqref="C28"/>
+      <selection activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.5546875" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
@@ -1098,16 +1107,30 @@
       <c r="C35" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="D35" s="3"/>
-      <c r="E35" s="3"/>
+      <c r="D35" s="2" t="s">
+        <v>52</v>
+      </c>
+      <c r="E35" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F35" s="3"/>
     </row>
     <row r="36" spans="1:6" x14ac:dyDescent="0.3">
-      <c r="A36" s="3"/>
-      <c r="B36" s="3"/>
-      <c r="C36" s="3"/>
-      <c r="D36" s="3"/>
-      <c r="E36" s="3"/>
+      <c r="A36" s="3" t="s">
+        <v>48</v>
+      </c>
+      <c r="B36" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="C36" s="3" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="E36" s="3" t="s">
+        <v>51</v>
+      </c>
       <c r="F36" s="3"/>
     </row>
     <row r="37" spans="1:6" x14ac:dyDescent="0.3">

</xml_diff>